<commit_message>
Realistic Prosthetics Expansion 수정
#686
</commit_message>
<xml_diff>
--- a/Data/Realistic Prosthetics Expansion - 1498483853/1498483853.xlsx
+++ b/Data/Realistic Prosthetics Expansion - 1498483853/1498483853.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.11\Realistic Prosthetics Expansion - 1498483853\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Realistic Prosthetics Expansion - 1498483853\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D7952C-C344-4C06-B7C7-3B4E49183B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB9E391-5481-4972-8AA1-9C3474226B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240416" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240417" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="401">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -968,66 +968,27 @@
     <t>An artifical stomach built by an archotech. Its internal workings are a mystery to all human minds.</t>
   </si>
   <si>
-    <t>초월공학이 제작한 인공 위. 그것의 내부 작동은 모든 인간의 마음에 미스터리입니다.</t>
-  </si>
-  <si>
     <t>초월공학 위</t>
   </si>
   <si>
-    <t>초월공학이 제작한 인공 척추입니다. 그것의 내부 작동은 모든 인간의 마음에 미스터리입니다.</t>
-  </si>
-  <si>
     <t>초월공학 척추</t>
   </si>
   <si>
-    <t>초월공학이 제작한 인공심장. 그것의 내부 작동은 모든 인간의 마음에 미스터리입니다.</t>
-  </si>
-  <si>
     <t>초월공학 심장</t>
   </si>
   <si>
-    <t>초월공학이 제작한 인공손. 두꺼운 활엽수 가지를 으스러뜨릴 만큼 강하고, 쌀알 위에 소네트를 쓸 만큼 정확합니다. 자연 살처럼 보이고 느껴지지만, 플라스틸보다 손상되기가 더 어렵습니다. 손상되더라도 시간이 지나면 저절로 복구됩니다. 그것의 내부 작동은 모든 인간의 마음에 미스터리입니다.</t>
-  </si>
-  <si>
     <t>초월공학 손</t>
   </si>
   <si>
-    <t>진보된 인공 폐. 합성 근육 섬유는 고급 미세막을 통해 산소를 끌어옵니다. 통합된 격자-먼지 치유 시스템이 자동으로 손상을 복구합니다. 거의 모든 면에서 생물학적 폐보다 낫습니다.</t>
-  </si>
-  <si>
     <t>생체공학 폐</t>
   </si>
   <si>
-    <t>진보된 인공신장. 강력한 나노 필터 세트가 혈류에서 거의 모든 독소를 효과적으로 제거합니다. 통합된 격자-먼지 치유 시스템이 모든 손상을 자동으로 복구합니다. 거의 모든 면에서 생물학적 신장보다 낫습니다.</t>
-  </si>
-  <si>
     <t>생체공학 신장</t>
   </si>
   <si>
-    <t>진보된 인공 간. 일련의 화학 합성기는 신체를 변화시키는 거의 모든 물질을 효율적으로 처리합니다. 통합된 격자-먼지 치유 시스템은 모든 손상을 자동으로 복구합니다. 거의 모든 면에서 생물학적 간보다 낫습니다.</t>
-  </si>
-  <si>
-    <t>생체 공 간</t>
-  </si>
-  <si>
-    <t>진보된 인공 발 입니다. 소음이 적은 미니 서보와 바이오겔 신경 링크는 뛰어난 균형감과 제어력을 제공합니다.  격자-분진 치유 시스템을 통해 손상을 복구할 수 있습니다. 거의 모든 면에서 생물학적 발보다 낫습니다.</t>
-  </si>
-  <si>
     <t>생체공학 발</t>
   </si>
   <si>
-    <t>진보된 인공 손 입니다. 격자-분진 치유 시스템은 그것이 손상으로부터 회복하도록 허용하는 반면, 소형 서보 배열은 놀라운 손재주를 줍니다. 그것은 거의 모든 면에서 생물학적 손보다 낫습니다</t>
-  </si>
-  <si>
-    <t>생체 공학 손</t>
-  </si>
-  <si>
-    <t>손가락이나 발가락을 모방할 수 있는 인공 보철물 입니다. 신경 인터페이스가 부족하지만 내부 관절의 복잡한 배열을 통해 자연스러운 움직임을 매우 설득력 있게 모방할 수 있습니다. 그래도 실제 손가락 발가락 보다는 못합니다.</t>
-  </si>
-  <si>
-    <t>손가락 발가락 보철물</t>
-  </si>
-  <si>
     <t>발 보철물. 신경 인터페이스가 부족하지만 내부 관절의 복잡한 배열을 통해 자연스러운 움직임을 매우 설득력 있게 모방할 수 있습니다. 그래도 실제 발보다는 못합니다.</t>
   </si>
   <si>
@@ -1040,147 +1001,9 @@
     <t>의수</t>
   </si>
   <si>
-    <t>초월공학 위장을 설치합니다.</t>
-  </si>
-  <si>
-    <t>초월공학 위장을 설치하세요.</t>
-  </si>
-  <si>
-    <t>초월공학 위장 설치하다</t>
-  </si>
-  <si>
-    <t>Archotech 척추를 설치합니다.</t>
-  </si>
-  <si>
-    <t>Archotech 척추를 설치하십시오.</t>
-  </si>
-  <si>
-    <t>초월공학 척추 설치</t>
-  </si>
-  <si>
-    <t>아르코테크 하트를 설치합니다.</t>
-  </si>
-  <si>
-    <t>아르코테크 하트를 설치하세요.</t>
-  </si>
-  <si>
-    <t>초월공학 심장 설치</t>
-  </si>
-  <si>
-    <t>아르코테크 핸드 설치.</t>
-  </si>
-  <si>
-    <t>아르코테크 핸드를 설치하세요.</t>
-  </si>
-  <si>
-    <t>초월공학 손 설치</t>
-  </si>
-  <si>
-    <t>뼈 수리</t>
-  </si>
-  <si>
-    <t>부서진 뼈를 수리하세요.</t>
-  </si>
-  <si>
-    <t>뼈를 고치다</t>
-  </si>
-  <si>
-    <t>생체공학 폐 설치.</t>
-  </si>
-  <si>
-    <t>생체공학 폐를 설치합니다.</t>
-  </si>
-  <si>
-    <t>생체공학 폐를 설치하다</t>
-  </si>
-  <si>
-    <t>생체공학 신장 설치.</t>
-  </si>
-  <si>
-    <t>생체공학 신장을 설치합니다.</t>
-  </si>
-  <si>
-    <t>생체공학 신장을 설치하다</t>
-  </si>
-  <si>
-    <t>생체 공학 간 설치.</t>
-  </si>
-  <si>
-    <t>생체공학 간을 설치합니다.</t>
-  </si>
-  <si>
-    <t>생체공학 간을 설치하다</t>
-  </si>
-  <si>
-    <t>생체공학 발을 설치합니다.</t>
-  </si>
-  <si>
-    <t>생체공학 발을 설치하다</t>
-  </si>
-  <si>
-    <t>바이오닉 핸드를 설치합니다.</t>
-  </si>
-  <si>
-    <t>생체공학 손을 설치합니다.</t>
-  </si>
-  <si>
-    <t>바이오닉 핸드를 설치하다</t>
-  </si>
-  <si>
-    <t>인공 코를 설치합니다.</t>
-  </si>
-  <si>
-    <t>인공 코를 설치하다</t>
-  </si>
-  <si>
-    <t>인공수지 설치.</t>
-  </si>
-  <si>
-    <t>인공 손가락을 설치합니다.</t>
-  </si>
-  <si>
-    <t>인공수지 설치</t>
-  </si>
-  <si>
-    <t>의족 설치.</t>
-  </si>
-  <si>
-    <t>의족을 설치합니다.</t>
-  </si>
-  <si>
-    <t>의족을 설치하다</t>
-  </si>
-  <si>
-    <t>의수 설치.</t>
-  </si>
-  <si>
-    <t>의수를 설치합니다.</t>
-  </si>
-  <si>
-    <t>의수를 설치하다</t>
-  </si>
-  <si>
-    <t>유리눈 설치.</t>
-  </si>
-  <si>
-    <t>유리 눈을 설치하십시오.</t>
-  </si>
-  <si>
-    <t>유리눈을 설치하다</t>
-  </si>
-  <si>
     <t>설치된 초월공학 위장.</t>
   </si>
   <si>
-    <t>설치된 아키텍 척추.</t>
-  </si>
-  <si>
-    <t>설치된 초월공학 심장입니다.</t>
-  </si>
-  <si>
-    <t>손</t>
-  </si>
-  <si>
     <t>설치된 초월공학 손.</t>
   </si>
   <si>
@@ -1208,33 +1031,18 @@
     <t>설치된 생체 공학 발.</t>
   </si>
   <si>
-    <t>생체 공학적 발</t>
-  </si>
-  <si>
     <t>주먹</t>
   </si>
   <si>
     <t>설치된 생체 공학 손.</t>
   </si>
   <si>
-    <t>생체 공학적 손</t>
-  </si>
-  <si>
     <t>설치된 인공 코.</t>
   </si>
   <si>
     <t>인공 코</t>
   </si>
   <si>
-    <t>설치된 보철물.</t>
-  </si>
-  <si>
-    <t>보철 손가락</t>
-  </si>
-  <si>
-    <t>설치된 의족입니다.</t>
-  </si>
-  <si>
     <t>설치된 의수.</t>
   </si>
   <si>
@@ -1242,6 +1050,196 @@
   </si>
   <si>
     <t>유리 눈</t>
+  </si>
+  <si>
+    <t>초월공학이 제작한 인공 위. 작동 원리는 수수께끼입니다.</t>
+  </si>
+  <si>
+    <t>초월공학이 제작한 인공 척추입니다. 작동 원리는 수수께끼입니다.</t>
+  </si>
+  <si>
+    <t>초월공학이 제작한 인공심장. 작동 원리는 수수께끼입니다.</t>
+  </si>
+  <si>
+    <t>초월공학이 제작한 인공손. 두꺼운 활엽수 가지를 으스러뜨릴 만큼 강하고, 쌀알 위에 소네트를 쓸 만큼 정확합니다. 자연 살처럼 보이고 느껴지지만, 플라스틸보다 손상되기가 더 어렵습니다. 손상되더라도 시간이 지나면 저절로 복구됩니다. 작동 원리는 수수께끼입니다.</t>
+  </si>
+  <si>
+    <t>첨단 인공 폐. 합성 근육 섬유는 고급 미세막을 통해 산소를 끌어옵니다. 통합된 격자-분진 치유 시스템이 자동으로 손상을 복구합니다. 거의 모든 면에서 생물학적 폐보다 낫습니다.</t>
+  </si>
+  <si>
+    <t>첨단 인공신장. 강력한 나노 필터 세트가 혈류에서 거의 모든 독소를 효과적으로 제거합니다. 통합된 격자-분진 치유 시스템이 모든 손상을 자동으로 복구합니다. 거의 모든 면에서 생물학적 신장보다 낫습니다.</t>
+  </si>
+  <si>
+    <t>첨단 인공 간. 일련의 화학 합성기는 신체를 변화시키는 거의 모든 물질을 효율적으로 처리합니다. 통합된 격자-분진 치유 시스템은 모든 손상을 자동으로 복구합니다. 거의 모든 면에서 생물학적 간보다 낫습니다.</t>
+  </si>
+  <si>
+    <t>첨단 인공 발 입니다. 소음이 적은 미니 서보와 바이오겔 신경 링크는 뛰어난 균형감과 제어력을 제공합니다. 격자-분진 치유 시스템을 통해 손상을 복구할 수 있습니다. 거의 모든 면에서 생물학적 발보다 낫습니다.</t>
+  </si>
+  <si>
+    <t>고급 인공 손 입니다. 소형 서보 어레이는 놀라운 민첩성을 제공하며, 격자-분진 치유 시스템을 통해 손상을 복구할 수 있습니다. 거의 모든 면에서 생물학적 손보다 낫습니다.</t>
+  </si>
+  <si>
+    <t>생체공학 손</t>
+  </si>
+  <si>
+    <t>손가락이나 발가락을 모방할 수 있는 인공 손가락입니다. 신경 인터페이스가 부족하지만 내부 관절의 복잡한 배열을 통해 자연스러운 움직임을 매우 설득력 있게 모방할 수 있습니다. 그래도 실제 숫자보다는 열등합니다.</t>
+  </si>
+  <si>
+    <t>보철 손,발가락</t>
+  </si>
+  <si>
+    <t>초월공학 위장을 이식합니다.</t>
+  </si>
+  <si>
+    <t>초월공학 위장 이식</t>
+  </si>
+  <si>
+    <t>초월공학 척추를 이식합니다.</t>
+  </si>
+  <si>
+    <t>초월공학 척추 이식</t>
+  </si>
+  <si>
+    <t>초월공학 심장을 이식합니다.</t>
+  </si>
+  <si>
+    <t>초월공학 심장 이식</t>
+  </si>
+  <si>
+    <t>초월공학 손을 이식합니다.</t>
+  </si>
+  <si>
+    <t>초월공학 손 이식</t>
+  </si>
+  <si>
+    <t>뼈 복원 중</t>
+  </si>
+  <si>
+    <t>부서진 뼈를 복원 합니다.</t>
+  </si>
+  <si>
+    <t>뼈 복원</t>
+  </si>
+  <si>
+    <t>생체공학 폐를 이식합니다.</t>
+  </si>
+  <si>
+    <t>생체공학 폐 이식</t>
+  </si>
+  <si>
+    <t>생체공학 신장을 이식합니다.</t>
+  </si>
+  <si>
+    <t>생체공학 신장 이식</t>
+  </si>
+  <si>
+    <t>생체공학 간을 이식합니다.</t>
+  </si>
+  <si>
+    <t>생체공학 간 이식</t>
+  </si>
+  <si>
+    <t>생체공학 발을 이식합니다.</t>
+  </si>
+  <si>
+    <t>생체공학 발 이식</t>
+  </si>
+  <si>
+    <t>생체공학 손을 이식합니다.</t>
+  </si>
+  <si>
+    <t>생체공학 손 이식</t>
+  </si>
+  <si>
+    <t>인공 코를 이식합니다.</t>
+  </si>
+  <si>
+    <t>인공 코 이식</t>
+  </si>
+  <si>
+    <t>인공 손,발가락 이식</t>
+  </si>
+  <si>
+    <t>의족을 이식합니다.</t>
+  </si>
+  <si>
+    <t>의족 이식</t>
+  </si>
+  <si>
+    <t>의수를 이식합니다.</t>
+  </si>
+  <si>
+    <t>의수 이식</t>
+  </si>
+  <si>
+    <t>유리 눈을 이식합니다.</t>
+  </si>
+  <si>
+    <t>유리눈 이식</t>
+  </si>
+  <si>
+    <t>설치된 초월공학 척추.</t>
+  </si>
+  <si>
+    <t>설치된 초월공학 심장 입니다.</t>
+  </si>
+  <si>
+    <t>설치된 의족.</t>
+  </si>
+  <si>
+    <t>설치된 인공 손, 발가락.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인공 손, 발가락</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유리눈 이식 중</t>
+  </si>
+  <si>
+    <t>의수 이식 중</t>
+  </si>
+  <si>
+    <t>의족 이식 중</t>
+  </si>
+  <si>
+    <t>인공 코 이식 중</t>
+  </si>
+  <si>
+    <t>생체공학 손을 이식 중</t>
+  </si>
+  <si>
+    <t>생체공학 발을 이식 중</t>
+  </si>
+  <si>
+    <t>생체 공학 간을 이식 중</t>
+  </si>
+  <si>
+    <t>생체 공학 신장을 이식 중</t>
+  </si>
+  <si>
+    <t>생체공학 폐 이식 중</t>
+  </si>
+  <si>
+    <t>초월공학 손 이식 중</t>
+  </si>
+  <si>
+    <t>초월공학 심장 이식 중</t>
+  </si>
+  <si>
+    <t>초월공학 척추 이식 중</t>
+  </si>
+  <si>
+    <t>초월공학 위장 이식 중</t>
+  </si>
+  <si>
+    <t>인공 손, 발가락을 이식합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인공 손, 발가락 이식 중</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1596,7 +1594,7 @@
   <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1644,7 +1642,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>402</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1661,7 +1659,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>402</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1678,7 +1676,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>401</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1695,7 +1693,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1712,7 +1710,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1729,7 +1727,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>400</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1746,7 +1744,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1763,7 +1761,7 @@
         <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -1780,7 +1778,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -1797,7 +1795,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -1814,7 +1812,7 @@
         <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>334</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1831,7 +1829,7 @@
         <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -1848,7 +1846,7 @@
         <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>396</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1865,7 +1863,7 @@
         <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>396</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -1882,7 +1880,7 @@
         <v>51</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>395</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -1899,7 +1897,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>394</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1916,7 +1914,7 @@
         <v>57</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>394</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1933,7 +1931,7 @@
         <v>60</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>393</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1950,7 +1948,7 @@
         <v>63</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>392</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1967,7 +1965,7 @@
         <v>66</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -1984,7 +1982,7 @@
         <v>69</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>391</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -2001,7 +1999,7 @@
         <v>72</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>390</v>
+        <v>331</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -2018,7 +2016,7 @@
         <v>75</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>389</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -2035,7 +2033,7 @@
         <v>78</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>388</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -2052,7 +2050,7 @@
         <v>81</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>387</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -2069,7 +2067,7 @@
         <v>84</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>386</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -2086,7 +2084,7 @@
         <v>87</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>386</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -2103,7 +2101,7 @@
         <v>90</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>385</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -2120,7 +2118,7 @@
         <v>93</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>384</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -2137,7 +2135,7 @@
         <v>96</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>384</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -2154,7 +2152,7 @@
         <v>99</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>383</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -2171,7 +2169,7 @@
         <v>102</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -2188,7 +2186,7 @@
         <v>105</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -2205,7 +2203,7 @@
         <v>108</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>382</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -2222,7 +2220,7 @@
         <v>63</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>381</v>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -2239,7 +2237,7 @@
         <v>113</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -2256,7 +2254,7 @@
         <v>116</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
@@ -2273,7 +2271,7 @@
         <v>119</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -2290,7 +2288,7 @@
         <v>122</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -2307,7 +2305,7 @@
         <v>125</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -2324,7 +2322,7 @@
         <v>128</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -2341,7 +2339,7 @@
         <v>131</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -2358,7 +2356,7 @@
         <v>134</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
@@ -2375,7 +2373,7 @@
         <v>137</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>378</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -2392,7 +2390,7 @@
         <v>141</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -2409,7 +2407,7 @@
         <v>144</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -2426,7 +2424,7 @@
         <v>147</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
@@ -2443,7 +2441,7 @@
         <v>150</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
@@ -2460,7 +2458,7 @@
         <v>153</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
@@ -2477,7 +2475,7 @@
         <v>156</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>372</v>
+        <v>387</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -2494,7 +2492,7 @@
         <v>159</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -2511,7 +2509,7 @@
         <v>162</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
@@ -2528,7 +2526,7 @@
         <v>165</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
@@ -2545,7 +2543,7 @@
         <v>168</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
@@ -2562,7 +2560,7 @@
         <v>171</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>367</v>
+        <v>399</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
@@ -2579,7 +2577,7 @@
         <v>174</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>366</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
@@ -2596,7 +2594,7 @@
         <v>177</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
@@ -2613,7 +2611,7 @@
         <v>180</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
@@ -2630,7 +2628,7 @@
         <v>183</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
@@ -2647,7 +2645,7 @@
         <v>186</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
@@ -2664,7 +2662,7 @@
         <v>189</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
@@ -2681,7 +2679,7 @@
         <v>192</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>361</v>
+        <v>390</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
@@ -2698,7 +2696,7 @@
         <v>195</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -2715,7 +2713,7 @@
         <v>198</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
@@ -2732,7 +2730,7 @@
         <v>201</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>359</v>
+        <v>391</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
@@ -2749,7 +2747,7 @@
         <v>204</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
@@ -2766,7 +2764,7 @@
         <v>207</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
@@ -2783,7 +2781,7 @@
         <v>210</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>356</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
@@ -2800,7 +2798,7 @@
         <v>213</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
@@ -2817,7 +2815,7 @@
         <v>216</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
@@ -2834,7 +2832,7 @@
         <v>219</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>353</v>
+        <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
@@ -2851,7 +2849,7 @@
         <v>222</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
@@ -2868,7 +2866,7 @@
         <v>225</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
@@ -2885,7 +2883,7 @@
         <v>228</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
@@ -2902,7 +2900,7 @@
         <v>231</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
@@ -2919,7 +2917,7 @@
         <v>234</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
@@ -2936,7 +2934,7 @@
         <v>237</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
@@ -2953,7 +2951,7 @@
         <v>240</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
@@ -2970,7 +2968,7 @@
         <v>243</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
@@ -2987,7 +2985,7 @@
         <v>246</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>344</v>
+        <v>395</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
@@ -3004,7 +3002,7 @@
         <v>249</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
@@ -3021,7 +3019,7 @@
         <v>252</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
@@ -3038,7 +3036,7 @@
         <v>255</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>341</v>
+        <v>396</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
@@ -3055,7 +3053,7 @@
         <v>258</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
@@ -3072,7 +3070,7 @@
         <v>261</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
@@ -3089,7 +3087,7 @@
         <v>264</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>338</v>
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
@@ -3106,7 +3104,7 @@
         <v>267</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
@@ -3123,7 +3121,7 @@
         <v>270</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
@@ -3140,7 +3138,7 @@
         <v>273</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>335</v>
+        <v>398</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
@@ -3157,7 +3155,7 @@
         <v>18</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
@@ -3174,7 +3172,7 @@
         <v>277</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
@@ -3191,7 +3189,7 @@
         <v>27</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
@@ -3208,7 +3206,7 @@
         <v>280</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
@@ -3225,7 +3223,7 @@
         <v>36</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
@@ -3242,7 +3240,7 @@
         <v>283</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
@@ -3259,7 +3257,7 @@
         <v>54</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
@@ -3276,7 +3274,7 @@
         <v>286</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
@@ -3293,7 +3291,7 @@
         <v>66</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
@@ -3310,7 +3308,7 @@
         <v>289</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
@@ -3327,7 +3325,7 @@
         <v>75</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
@@ -3344,7 +3342,7 @@
         <v>292</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>323</v>
+        <v>345</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
@@ -3361,7 +3359,7 @@
         <v>84</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.45">
@@ -3378,7 +3376,7 @@
         <v>295</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>321</v>
+        <v>344</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
@@ -3395,7 +3393,7 @@
         <v>93</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
@@ -3412,7 +3410,7 @@
         <v>298</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>319</v>
+        <v>343</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
@@ -3429,7 +3427,7 @@
         <v>102</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
@@ -3446,7 +3444,7 @@
         <v>301</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.45">
@@ -3463,7 +3461,7 @@
         <v>113</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.45">
@@ -3480,7 +3478,7 @@
         <v>304</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.45">
@@ -3497,7 +3495,7 @@
         <v>122</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
@@ -3514,7 +3512,7 @@
         <v>307</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>313</v>
+        <v>340</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.45">
@@ -3531,7 +3529,7 @@
         <v>131</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
@@ -3548,7 +3546,7 @@
         <v>310</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>311</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>